<commit_message>
cp offset test getting ready to parallelize
</commit_message>
<xml_diff>
--- a/studies/adjoint_studies/central_diff_norm_cp_offset/results/safety_test_11_10_cp_offsets_norms_vs_cp_offset_data.xlsx
+++ b/studies/adjoint_studies/central_diff_norm_cp_offset/results/safety_test_11_10_cp_offsets_norms_vs_cp_offset_data.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan\git-repos\MachLine\studies\adjoint_studies\central_diff_norm_cp_offset\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01BBD9F-7DED-44B5-9612-AD1CE4568F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9923760D-2C6C-4758-8BE0-4B217EBCC7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="26">
   <si>
     <t>Step Size</t>
   </si>
@@ -62,6 +75,42 @@
   </si>
   <si>
     <t>Adjoint</t>
+  </si>
+  <si>
+    <t># runs per CD</t>
+  </si>
+  <si>
+    <t>ryzen run time[s]</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>parallel</t>
+  </si>
+  <si>
+    <t>ryzen cores</t>
+  </si>
+  <si>
+    <t>total run time</t>
+  </si>
+  <si>
+    <t>in hours</t>
+  </si>
+  <si>
+    <t>in seconds</t>
+  </si>
+  <si>
+    <t>in days</t>
+  </si>
+  <si>
+    <t># cp offsets</t>
+  </si>
+  <si>
+    <t># step sizes</t>
+  </si>
+  <si>
+    <t>total # of runs</t>
   </si>
 </sst>
 </file>
@@ -149,8 +198,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>276774</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>614704</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>102589</xdr:rowOff>
     </xdr:to>
@@ -473,13 +522,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -762,7 +815,7 @@
         <v>31539745.754817922</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -779,7 +832,7 @@
         <v>221532.29036162069</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -796,7 +849,7 @@
         <v>5254.1920796379327</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -812,8 +865,11 @@
       <c r="E19">
         <v>49.061694652028862</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="O19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -829,8 +885,20 @@
       <c r="E20">
         <v>9.6273556853423141</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K20" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" t="s">
+        <v>16</v>
+      </c>
+      <c r="P20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -846,8 +914,21 @@
       <c r="E21">
         <v>4854101292.9064569</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>32</v>
+      </c>
+      <c r="M21">
+        <f>1190*6</f>
+        <v>7140</v>
+      </c>
+      <c r="O21">
+        <v>3.9</v>
+      </c>
+      <c r="P21">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -864,7 +945,7 @@
         <v>18835907.784770239</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -880,8 +961,17 @@
       <c r="E23">
         <v>94320087.16694878</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" t="s">
+        <v>25</v>
+      </c>
+      <c r="O23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -897,8 +987,21 @@
       <c r="E24">
         <v>99682548.774113268</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K24">
+        <v>10</v>
+      </c>
+      <c r="M24">
+        <f>M21*K24*K27</f>
+        <v>499800</v>
+      </c>
+      <c r="O24" t="s">
+        <v>16</v>
+      </c>
+      <c r="P24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -914,8 +1017,19 @@
       <c r="E25">
         <v>277955716.51035529</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="O25">
+        <f>M21*K24*K27*O21/32</f>
+        <v>60913.125</v>
+      </c>
+      <c r="P25">
+        <f>M21*K24*K27*P21</f>
+        <v>649740</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -931,8 +1045,22 @@
       <c r="E26">
         <v>31539745.754817922</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K26" t="s">
+        <v>24</v>
+      </c>
+      <c r="O26">
+        <f>O25/3600</f>
+        <v>16.920312500000001</v>
+      </c>
+      <c r="P26">
+        <f>P25/3600</f>
+        <v>180.48333333333332</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -948,8 +1076,22 @@
       <c r="E27">
         <v>221532.29036162069</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>7</v>
+      </c>
+      <c r="O27">
+        <f>O26/24</f>
+        <v>0.70501302083333339</v>
+      </c>
+      <c r="P27">
+        <f>P26/24</f>
+        <v>7.520138888888888</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -966,7 +1108,7 @@
         <v>5254.1920796379327</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -983,7 +1125,7 @@
         <v>49.061694652028862</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1000,7 +1142,7 @@
         <v>9.6273556853423141</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1017,7 +1159,7 @@
         <v>4854101292.9064569</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
robust cp dir input changed
</commit_message>
<xml_diff>
--- a/studies/adjoint_studies/central_diff_norm_cp_offset/results/safety_test_11_10_cp_offsets_norms_vs_cp_offset_data.xlsx
+++ b/studies/adjoint_studies/central_diff_norm_cp_offset/results/safety_test_11_10_cp_offsets_norms_vs_cp_offset_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan\git-repos\MachLine\studies\adjoint_studies\central_diff_norm_cp_offset\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C1EEBD-C6A1-4DFF-A3B7-7DBF5E156BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED12939F-A416-4235-B891-3ED65A4AAD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2316" yWindow="2328" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39360" yWindow="4230" windowWidth="15120" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <t>total # of runs</t>
   </si>
   <si>
-    <t>started 1:00 am Thursday oct 17</t>
+    <t>started noon Thursday oct 17</t>
   </si>
 </sst>
 </file>
@@ -202,9 +202,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>614704</xdr:colOff>
+      <xdr:colOff>626134</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>102589</xdr:rowOff>
+      <xdr:rowOff>98779</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="I18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,14 +918,14 @@
         <v>4854101292.9064569</v>
       </c>
       <c r="K21">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="M21">
         <f>1190*6</f>
         <v>7140</v>
       </c>
       <c r="O21">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="P21">
         <v>1.3</v>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="O25">
         <f>M21*K24*K27*O21/K21</f>
-        <v>299880</v>
+        <v>208250</v>
       </c>
       <c r="P25">
         <f>M21*K24*K27*P21</f>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="O26">
         <f>O25/3600</f>
-        <v>83.3</v>
+        <v>57.847222222222221</v>
       </c>
       <c r="P26">
         <f>P25/3600</f>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="O27">
         <f>O26/24</f>
-        <v>3.4708333333333332</v>
+        <v>2.410300925925926</v>
       </c>
       <c r="P27">
         <f>P26/24</f>
@@ -1129,6 +1129,9 @@
       </c>
       <c r="E29">
         <v>49.061694652028862</v>
+      </c>
+      <c r="M29">
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>